<commit_message>
planning et plan architecture et uml
</commit_message>
<xml_diff>
--- a/planning_133.xlsx
+++ b/planning_133.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\133_Memory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FE5EB0-C06D-4AE5-A6EB-746467A826C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79361B1-A5AB-4F9A-A862-A99DE16F51FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>Tâches</t>
   </si>
@@ -1005,6 +1005,96 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1032,21 +1122,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1055,81 +1130,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1479,8 +1479,8 @@
   </sheetPr>
   <dimension ref="A1:AM43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1491,40 +1491,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91"/>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="91"/>
-      <c r="Z1" s="91"/>
-      <c r="AA1" s="91"/>
-      <c r="AB1" s="91"/>
-      <c r="AC1" s="91"/>
-      <c r="AD1" s="91"/>
-      <c r="AE1" s="91"/>
-      <c r="AF1" s="91"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="83"/>
       <c r="AG1" s="14"/>
       <c r="AH1" s="14"/>
       <c r="AI1" s="14"/>
@@ -1537,26 +1537,26 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="104" t="s">
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="106" t="s">
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="106"/>
+      <c r="O2" s="102"/>
       <c r="P2" s="32"/>
       <c r="Q2" s="32"/>
       <c r="R2" s="32"/>
@@ -1583,20 +1583,20 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
       <c r="N3" s="38"/>
       <c r="O3" s="38"/>
       <c r="P3" s="38"/>
@@ -1622,47 +1622,47 @@
       <c r="AM3" s="32"/>
     </row>
     <row r="4" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="95" t="s">
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="100" t="s">
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="O4" s="101"/>
-      <c r="P4" s="101"/>
-      <c r="Q4" s="101"/>
-      <c r="R4" s="101"/>
-      <c r="S4" s="102"/>
+      <c r="O4" s="97"/>
+      <c r="P4" s="97"/>
+      <c r="Q4" s="97"/>
+      <c r="R4" s="97"/>
+      <c r="S4" s="98"/>
       <c r="T4" s="16"/>
-      <c r="U4" s="92" t="s">
+      <c r="U4" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="V4" s="93"/>
-      <c r="W4" s="93"/>
-      <c r="X4" s="93"/>
-      <c r="Y4" s="93"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="92" t="s">
+      <c r="V4" s="85"/>
+      <c r="W4" s="85"/>
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="AB4" s="93"/>
-      <c r="AC4" s="93"/>
-      <c r="AD4" s="93"/>
-      <c r="AE4" s="93"/>
-      <c r="AF4" s="94"/>
+      <c r="AB4" s="85"/>
+      <c r="AC4" s="85"/>
+      <c r="AD4" s="85"/>
+      <c r="AE4" s="85"/>
+      <c r="AF4" s="86"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="33"/>
       <c r="AI4" s="33"/>
@@ -1675,57 +1675,57 @@
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="98">
+      <c r="B5" s="90">
         <v>45008</v>
       </c>
-      <c r="C5" s="99"/>
-      <c r="D5" s="87">
+      <c r="C5" s="91"/>
+      <c r="D5" s="92">
         <v>45009</v>
       </c>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="85">
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="95">
         <v>45015</v>
       </c>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83">
+      <c r="I5" s="93"/>
+      <c r="J5" s="93">
         <v>45016</v>
       </c>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="85">
+      <c r="K5" s="93"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="95">
         <v>45023</v>
       </c>
-      <c r="O5" s="86"/>
-      <c r="P5" s="87">
+      <c r="O5" s="103"/>
+      <c r="P5" s="92">
         <v>45024</v>
       </c>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="84"/>
+      <c r="Q5" s="93"/>
+      <c r="R5" s="93"/>
+      <c r="S5" s="94"/>
       <c r="T5" s="15"/>
-      <c r="U5" s="85">
+      <c r="U5" s="95">
         <v>45043</v>
       </c>
-      <c r="V5" s="86"/>
-      <c r="W5" s="87">
+      <c r="V5" s="103"/>
+      <c r="W5" s="92">
         <v>45044</v>
       </c>
-      <c r="X5" s="83"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="84"/>
-      <c r="AA5" s="85">
+      <c r="X5" s="93"/>
+      <c r="Y5" s="93"/>
+      <c r="Z5" s="94"/>
+      <c r="AA5" s="95">
         <v>45050</v>
       </c>
-      <c r="AB5" s="86"/>
-      <c r="AC5" s="87">
+      <c r="AB5" s="103"/>
+      <c r="AC5" s="92">
         <v>45051</v>
       </c>
-      <c r="AD5" s="83"/>
-      <c r="AE5" s="83"/>
-      <c r="AF5" s="84"/>
+      <c r="AD5" s="93"/>
+      <c r="AE5" s="93"/>
+      <c r="AF5" s="94"/>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
       <c r="AI5" s="4"/>
@@ -1768,13 +1768,13 @@
       <c r="M6" s="20"/>
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
-      <c r="P6" s="74" t="s">
+      <c r="P6" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="Q6" s="75"/>
-      <c r="R6" s="75"/>
-      <c r="S6" s="76"/>
-      <c r="T6" s="88" t="s">
+      <c r="Q6" s="105"/>
+      <c r="R6" s="105"/>
+      <c r="S6" s="106"/>
+      <c r="T6" s="113" t="s">
         <v>13</v>
       </c>
       <c r="U6" s="19"/>
@@ -1809,11 +1809,11 @@
       <c r="M7" s="24"/>
       <c r="N7" s="21"/>
       <c r="O7" s="22"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="78"/>
-      <c r="R7" s="78"/>
-      <c r="S7" s="79"/>
-      <c r="T7" s="89"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="108"/>
+      <c r="R7" s="108"/>
+      <c r="S7" s="109"/>
+      <c r="T7" s="114"/>
       <c r="U7" s="21"/>
       <c r="V7" s="22"/>
       <c r="W7" s="21"/>
@@ -1848,11 +1848,11 @@
       <c r="M8" s="24"/>
       <c r="N8" s="21"/>
       <c r="O8" s="22"/>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="78"/>
-      <c r="S8" s="79"/>
-      <c r="T8" s="89"/>
+      <c r="P8" s="107"/>
+      <c r="Q8" s="108"/>
+      <c r="R8" s="108"/>
+      <c r="S8" s="109"/>
+      <c r="T8" s="114"/>
       <c r="U8" s="21"/>
       <c r="V8" s="22"/>
       <c r="W8" s="21"/>
@@ -1887,11 +1887,11 @@
       <c r="M9" s="24"/>
       <c r="N9" s="21"/>
       <c r="O9" s="22"/>
-      <c r="P9" s="77"/>
-      <c r="Q9" s="78"/>
-      <c r="R9" s="78"/>
-      <c r="S9" s="79"/>
-      <c r="T9" s="89"/>
+      <c r="P9" s="107"/>
+      <c r="Q9" s="108"/>
+      <c r="R9" s="108"/>
+      <c r="S9" s="109"/>
+      <c r="T9" s="114"/>
       <c r="U9" s="21"/>
       <c r="V9" s="22"/>
       <c r="W9" s="21"/>
@@ -1920,15 +1920,17 @@
       <c r="I10" s="22"/>
       <c r="J10" s="21"/>
       <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
+      <c r="L10" s="64" t="s">
+        <v>12</v>
+      </c>
       <c r="M10" s="24"/>
       <c r="N10" s="21"/>
       <c r="O10" s="22"/>
-      <c r="P10" s="77"/>
-      <c r="Q10" s="78"/>
-      <c r="R10" s="78"/>
-      <c r="S10" s="79"/>
-      <c r="T10" s="89"/>
+      <c r="P10" s="107"/>
+      <c r="Q10" s="108"/>
+      <c r="R10" s="108"/>
+      <c r="S10" s="109"/>
+      <c r="T10" s="114"/>
       <c r="U10" s="21"/>
       <c r="V10" s="22"/>
       <c r="W10" s="21"/>
@@ -1963,11 +1965,11 @@
       <c r="M11" s="24"/>
       <c r="N11" s="21"/>
       <c r="O11" s="22"/>
-      <c r="P11" s="77"/>
-      <c r="Q11" s="78"/>
-      <c r="R11" s="78"/>
-      <c r="S11" s="79"/>
-      <c r="T11" s="89"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="108"/>
+      <c r="R11" s="108"/>
+      <c r="S11" s="109"/>
+      <c r="T11" s="114"/>
       <c r="U11" s="21"/>
       <c r="V11" s="22"/>
       <c r="W11" s="21"/>
@@ -2002,11 +2004,11 @@
       <c r="M12" s="24"/>
       <c r="N12" s="21"/>
       <c r="O12" s="22"/>
-      <c r="P12" s="77"/>
-      <c r="Q12" s="78"/>
-      <c r="R12" s="78"/>
-      <c r="S12" s="79"/>
-      <c r="T12" s="89"/>
+      <c r="P12" s="107"/>
+      <c r="Q12" s="108"/>
+      <c r="R12" s="108"/>
+      <c r="S12" s="109"/>
+      <c r="T12" s="114"/>
       <c r="U12" s="21"/>
       <c r="V12" s="22"/>
       <c r="W12" s="21"/>
@@ -2034,16 +2036,16 @@
       <c r="H13" s="21"/>
       <c r="I13" s="22"/>
       <c r="J13" s="21"/>
-      <c r="K13" s="108"/>
+      <c r="K13" s="75"/>
       <c r="L13" s="64"/>
       <c r="M13" s="65"/>
       <c r="N13" s="21"/>
       <c r="O13" s="22"/>
-      <c r="P13" s="77"/>
-      <c r="Q13" s="78"/>
-      <c r="R13" s="78"/>
-      <c r="S13" s="79"/>
-      <c r="T13" s="89"/>
+      <c r="P13" s="107"/>
+      <c r="Q13" s="108"/>
+      <c r="R13" s="108"/>
+      <c r="S13" s="109"/>
+      <c r="T13" s="114"/>
       <c r="U13" s="21"/>
       <c r="V13" s="22"/>
       <c r="W13" s="21"/>
@@ -2078,11 +2080,11 @@
       <c r="M14" s="24"/>
       <c r="N14" s="21"/>
       <c r="O14" s="22"/>
-      <c r="P14" s="77"/>
-      <c r="Q14" s="78"/>
-      <c r="R14" s="78"/>
-      <c r="S14" s="79"/>
-      <c r="T14" s="89"/>
+      <c r="P14" s="107"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="109"/>
+      <c r="T14" s="114"/>
       <c r="U14" s="21"/>
       <c r="V14" s="22"/>
       <c r="W14" s="21"/>
@@ -2117,11 +2119,11 @@
       <c r="M15" s="24"/>
       <c r="N15" s="21"/>
       <c r="O15" s="22"/>
-      <c r="P15" s="77"/>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="78"/>
-      <c r="S15" s="79"/>
-      <c r="T15" s="89"/>
+      <c r="P15" s="107"/>
+      <c r="Q15" s="108"/>
+      <c r="R15" s="108"/>
+      <c r="S15" s="109"/>
+      <c r="T15" s="114"/>
       <c r="U15" s="21"/>
       <c r="V15" s="22"/>
       <c r="W15" s="21"/>
@@ -2149,16 +2151,16 @@
       <c r="H16" s="21"/>
       <c r="I16" s="22"/>
       <c r="J16" s="21"/>
-      <c r="K16" s="108"/>
+      <c r="K16" s="75"/>
       <c r="L16" s="64"/>
       <c r="M16" s="71"/>
       <c r="N16" s="21"/>
       <c r="O16" s="22"/>
-      <c r="P16" s="77"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="78"/>
-      <c r="S16" s="79"/>
-      <c r="T16" s="89"/>
+      <c r="P16" s="107"/>
+      <c r="Q16" s="108"/>
+      <c r="R16" s="108"/>
+      <c r="S16" s="109"/>
+      <c r="T16" s="114"/>
       <c r="U16" s="21"/>
       <c r="V16" s="22"/>
       <c r="W16" s="21"/>
@@ -2191,11 +2193,11 @@
       <c r="M17" s="25"/>
       <c r="N17" s="21"/>
       <c r="O17" s="22"/>
-      <c r="P17" s="77"/>
-      <c r="Q17" s="78"/>
-      <c r="R17" s="78"/>
-      <c r="S17" s="79"/>
-      <c r="T17" s="89"/>
+      <c r="P17" s="107"/>
+      <c r="Q17" s="108"/>
+      <c r="R17" s="108"/>
+      <c r="S17" s="109"/>
+      <c r="T17" s="114"/>
       <c r="U17" s="21"/>
       <c r="V17" s="22"/>
       <c r="W17" s="21"/>
@@ -2228,13 +2230,13 @@
       <c r="M18" s="25"/>
       <c r="N18" s="21"/>
       <c r="O18" s="22"/>
-      <c r="P18" s="77"/>
-      <c r="Q18" s="78"/>
-      <c r="R18" s="78"/>
-      <c r="S18" s="79"/>
-      <c r="T18" s="89"/>
-      <c r="U18" s="109"/>
-      <c r="V18" s="110"/>
+      <c r="P18" s="107"/>
+      <c r="Q18" s="108"/>
+      <c r="R18" s="108"/>
+      <c r="S18" s="109"/>
+      <c r="T18" s="114"/>
+      <c r="U18" s="76"/>
+      <c r="V18" s="77"/>
       <c r="W18" s="21"/>
       <c r="X18" s="22"/>
       <c r="Y18" s="22"/>
@@ -2265,17 +2267,17 @@
       <c r="M19" s="25"/>
       <c r="N19" s="21"/>
       <c r="O19" s="22"/>
-      <c r="P19" s="77"/>
-      <c r="Q19" s="78"/>
-      <c r="R19" s="78"/>
-      <c r="S19" s="79"/>
-      <c r="T19" s="89"/>
+      <c r="P19" s="107"/>
+      <c r="Q19" s="108"/>
+      <c r="R19" s="108"/>
+      <c r="S19" s="109"/>
+      <c r="T19" s="114"/>
       <c r="U19" s="21"/>
       <c r="V19" s="22"/>
       <c r="W19" s="21"/>
       <c r="X19" s="22"/>
-      <c r="Y19" s="110"/>
-      <c r="Z19" s="114"/>
+      <c r="Y19" s="77"/>
+      <c r="Z19" s="81"/>
       <c r="AA19" s="21"/>
       <c r="AB19" s="22"/>
       <c r="AC19" s="21"/>
@@ -2300,13 +2302,13 @@
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
       <c r="M20" s="25"/>
-      <c r="N20" s="109"/>
-      <c r="O20" s="110"/>
-      <c r="P20" s="77"/>
-      <c r="Q20" s="78"/>
-      <c r="R20" s="78"/>
-      <c r="S20" s="79"/>
-      <c r="T20" s="89"/>
+      <c r="N20" s="76"/>
+      <c r="O20" s="77"/>
+      <c r="P20" s="107"/>
+      <c r="Q20" s="108"/>
+      <c r="R20" s="108"/>
+      <c r="S20" s="109"/>
+      <c r="T20" s="114"/>
       <c r="U20" s="21"/>
       <c r="V20" s="22"/>
       <c r="X20" s="22"/>
@@ -2338,17 +2340,17 @@
       <c r="M21" s="25"/>
       <c r="N21" s="21"/>
       <c r="O21" s="22"/>
-      <c r="P21" s="77"/>
-      <c r="Q21" s="78"/>
-      <c r="R21" s="78"/>
-      <c r="S21" s="79"/>
-      <c r="T21" s="89"/>
+      <c r="P21" s="107"/>
+      <c r="Q21" s="108"/>
+      <c r="R21" s="108"/>
+      <c r="S21" s="109"/>
+      <c r="T21" s="114"/>
       <c r="U21" s="21"/>
       <c r="V21" s="22"/>
       <c r="W21" s="21"/>
       <c r="X21" s="22"/>
-      <c r="Y21" s="110"/>
-      <c r="Z21" s="114"/>
+      <c r="Y21" s="77"/>
+      <c r="Z21" s="81"/>
       <c r="AA21" s="21"/>
       <c r="AB21" s="22"/>
       <c r="AC21" s="21"/>
@@ -2373,13 +2375,13 @@
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
       <c r="M22" s="25"/>
-      <c r="N22" s="109"/>
-      <c r="O22" s="110"/>
-      <c r="P22" s="77"/>
-      <c r="Q22" s="78"/>
-      <c r="R22" s="78"/>
-      <c r="S22" s="79"/>
-      <c r="T22" s="89"/>
+      <c r="N22" s="76"/>
+      <c r="O22" s="77"/>
+      <c r="P22" s="107"/>
+      <c r="Q22" s="108"/>
+      <c r="R22" s="108"/>
+      <c r="S22" s="109"/>
+      <c r="T22" s="114"/>
       <c r="U22" s="21"/>
       <c r="V22" s="22"/>
       <c r="W22" s="21"/>
@@ -2412,11 +2414,11 @@
       <c r="M23" s="25"/>
       <c r="N23" s="21"/>
       <c r="O23" s="22"/>
-      <c r="P23" s="77"/>
-      <c r="Q23" s="78"/>
-      <c r="R23" s="78"/>
-      <c r="S23" s="79"/>
-      <c r="T23" s="89"/>
+      <c r="P23" s="107"/>
+      <c r="Q23" s="108"/>
+      <c r="R23" s="108"/>
+      <c r="S23" s="109"/>
+      <c r="T23" s="114"/>
       <c r="U23" s="21"/>
       <c r="V23" s="22"/>
       <c r="W23" s="21"/>
@@ -2449,16 +2451,16 @@
       <c r="M24" s="25"/>
       <c r="N24" s="21"/>
       <c r="O24" s="22"/>
-      <c r="P24" s="77"/>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="78"/>
-      <c r="S24" s="79"/>
-      <c r="T24" s="89"/>
+      <c r="P24" s="107"/>
+      <c r="Q24" s="108"/>
+      <c r="R24" s="108"/>
+      <c r="S24" s="109"/>
+      <c r="T24" s="114"/>
       <c r="U24" s="21"/>
       <c r="V24" s="22"/>
-      <c r="W24" s="112"/>
-      <c r="X24" s="111"/>
-      <c r="Y24" s="111"/>
+      <c r="W24" s="79"/>
+      <c r="X24" s="78"/>
+      <c r="Y24" s="78"/>
       <c r="Z24" s="25"/>
       <c r="AA24" s="21"/>
       <c r="AB24" s="22"/>
@@ -2486,19 +2488,19 @@
       <c r="M25" s="25"/>
       <c r="N25" s="21"/>
       <c r="O25" s="22"/>
-      <c r="P25" s="77"/>
-      <c r="Q25" s="78"/>
-      <c r="R25" s="78"/>
-      <c r="S25" s="79"/>
-      <c r="T25" s="89"/>
+      <c r="P25" s="107"/>
+      <c r="Q25" s="108"/>
+      <c r="R25" s="108"/>
+      <c r="S25" s="109"/>
+      <c r="T25" s="114"/>
       <c r="U25" s="21"/>
       <c r="V25" s="22"/>
       <c r="W25" s="21"/>
       <c r="X25" s="22"/>
       <c r="Y25" s="22"/>
-      <c r="Z25" s="113"/>
-      <c r="AA25" s="112"/>
-      <c r="AB25" s="111"/>
+      <c r="Z25" s="80"/>
+      <c r="AA25" s="79"/>
+      <c r="AB25" s="78"/>
       <c r="AC25" s="21"/>
       <c r="AD25" s="22"/>
       <c r="AE25" s="22"/>
@@ -2522,14 +2524,14 @@
       <c r="L26" s="22"/>
       <c r="M26" s="23"/>
       <c r="N26" s="21"/>
-      <c r="O26" s="111"/>
-      <c r="P26" s="77"/>
-      <c r="Q26" s="78"/>
-      <c r="R26" s="78"/>
-      <c r="S26" s="79"/>
-      <c r="T26" s="89"/>
-      <c r="U26" s="112"/>
-      <c r="V26" s="111"/>
+      <c r="O26" s="78"/>
+      <c r="P26" s="107"/>
+      <c r="Q26" s="108"/>
+      <c r="R26" s="108"/>
+      <c r="S26" s="109"/>
+      <c r="T26" s="114"/>
+      <c r="U26" s="79"/>
+      <c r="V26" s="78"/>
       <c r="W26" s="21"/>
       <c r="X26" s="22"/>
       <c r="Y26" s="22"/>
@@ -2557,14 +2559,14 @@
       <c r="J27" s="21"/>
       <c r="K27" s="22"/>
       <c r="L27" s="22"/>
-      <c r="M27" s="107"/>
+      <c r="M27" s="74"/>
       <c r="N27" s="21"/>
       <c r="O27" s="22"/>
-      <c r="P27" s="77"/>
-      <c r="Q27" s="78"/>
-      <c r="R27" s="78"/>
-      <c r="S27" s="79"/>
-      <c r="T27" s="89"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="108"/>
+      <c r="R27" s="108"/>
+      <c r="S27" s="109"/>
+      <c r="T27" s="114"/>
       <c r="U27" s="21"/>
       <c r="V27" s="22"/>
       <c r="W27" s="21"/>
@@ -2597,19 +2599,19 @@
       <c r="M28" s="24"/>
       <c r="N28" s="21"/>
       <c r="O28" s="22"/>
-      <c r="P28" s="77"/>
-      <c r="Q28" s="78"/>
-      <c r="R28" s="78"/>
-      <c r="S28" s="79"/>
-      <c r="T28" s="89"/>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="108"/>
+      <c r="R28" s="108"/>
+      <c r="S28" s="109"/>
+      <c r="T28" s="114"/>
       <c r="U28" s="21"/>
       <c r="V28" s="22"/>
       <c r="W28" s="21"/>
       <c r="X28" s="22"/>
       <c r="Y28" s="22"/>
-      <c r="Z28" s="107"/>
-      <c r="AA28" s="112"/>
-      <c r="AB28" s="111"/>
+      <c r="Z28" s="74"/>
+      <c r="AA28" s="79"/>
+      <c r="AB28" s="78"/>
       <c r="AC28" s="21"/>
       <c r="AD28" s="22"/>
       <c r="AE28" s="22"/>
@@ -2633,14 +2635,14 @@
       <c r="L29" s="22"/>
       <c r="M29" s="24"/>
       <c r="N29" s="21"/>
-      <c r="O29" s="111"/>
-      <c r="P29" s="77"/>
-      <c r="Q29" s="78"/>
-      <c r="R29" s="78"/>
-      <c r="S29" s="79"/>
-      <c r="T29" s="89"/>
-      <c r="U29" s="112"/>
-      <c r="V29" s="111"/>
+      <c r="O29" s="78"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="108"/>
+      <c r="R29" s="108"/>
+      <c r="S29" s="109"/>
+      <c r="T29" s="114"/>
+      <c r="U29" s="79"/>
+      <c r="V29" s="78"/>
       <c r="W29" s="21"/>
       <c r="X29" s="22"/>
       <c r="Y29" s="22"/>
@@ -2668,14 +2670,14 @@
       <c r="J30" s="21"/>
       <c r="K30" s="22"/>
       <c r="L30" s="22"/>
-      <c r="M30" s="107"/>
+      <c r="M30" s="74"/>
       <c r="N30" s="21"/>
       <c r="O30" s="22"/>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="78"/>
-      <c r="R30" s="78"/>
-      <c r="S30" s="79"/>
-      <c r="T30" s="89"/>
+      <c r="P30" s="107"/>
+      <c r="Q30" s="108"/>
+      <c r="R30" s="108"/>
+      <c r="S30" s="109"/>
+      <c r="T30" s="114"/>
       <c r="U30" s="21"/>
       <c r="V30" s="22"/>
       <c r="W30" s="21"/>
@@ -2708,11 +2710,11 @@
       <c r="M31" s="24"/>
       <c r="N31" s="21"/>
       <c r="O31" s="22"/>
-      <c r="P31" s="77"/>
-      <c r="Q31" s="78"/>
-      <c r="R31" s="78"/>
-      <c r="S31" s="79"/>
-      <c r="T31" s="89"/>
+      <c r="P31" s="107"/>
+      <c r="Q31" s="108"/>
+      <c r="R31" s="108"/>
+      <c r="S31" s="109"/>
+      <c r="T31" s="114"/>
       <c r="U31" s="21"/>
       <c r="V31" s="22"/>
       <c r="W31" s="21"/>
@@ -2745,11 +2747,11 @@
       <c r="M32" s="24"/>
       <c r="N32" s="21"/>
       <c r="O32" s="22"/>
-      <c r="P32" s="77"/>
-      <c r="Q32" s="78"/>
-      <c r="R32" s="78"/>
-      <c r="S32" s="79"/>
-      <c r="T32" s="89"/>
+      <c r="P32" s="107"/>
+      <c r="Q32" s="108"/>
+      <c r="R32" s="108"/>
+      <c r="S32" s="109"/>
+      <c r="T32" s="114"/>
       <c r="U32" s="21"/>
       <c r="V32" s="22"/>
       <c r="W32" s="21"/>
@@ -2758,7 +2760,7 @@
       <c r="Z32" s="24"/>
       <c r="AA32" s="21"/>
       <c r="AB32" s="22"/>
-      <c r="AC32" s="115"/>
+      <c r="AC32" s="82"/>
       <c r="AD32" s="70"/>
       <c r="AE32" s="22"/>
       <c r="AF32" s="24"/>
@@ -2782,11 +2784,11 @@
       <c r="M33" s="24"/>
       <c r="N33" s="21"/>
       <c r="O33" s="22"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="78"/>
-      <c r="R33" s="78"/>
-      <c r="S33" s="79"/>
-      <c r="T33" s="89"/>
+      <c r="P33" s="107"/>
+      <c r="Q33" s="108"/>
+      <c r="R33" s="108"/>
+      <c r="S33" s="109"/>
+      <c r="T33" s="114"/>
       <c r="U33" s="21"/>
       <c r="V33" s="22"/>
       <c r="W33" s="21"/>
@@ -2795,7 +2797,7 @@
       <c r="Z33" s="24"/>
       <c r="AA33" s="21"/>
       <c r="AB33" s="22"/>
-      <c r="AC33" s="115"/>
+      <c r="AC33" s="82"/>
       <c r="AD33" s="70"/>
       <c r="AE33" s="22"/>
       <c r="AF33" s="24"/>
@@ -2819,11 +2821,11 @@
       <c r="M34" s="24"/>
       <c r="N34" s="21"/>
       <c r="O34" s="22"/>
-      <c r="P34" s="77"/>
-      <c r="Q34" s="78"/>
-      <c r="R34" s="78"/>
-      <c r="S34" s="79"/>
-      <c r="T34" s="89"/>
+      <c r="P34" s="107"/>
+      <c r="Q34" s="108"/>
+      <c r="R34" s="108"/>
+      <c r="S34" s="109"/>
+      <c r="T34" s="114"/>
       <c r="U34" s="21"/>
       <c r="V34" s="22"/>
       <c r="W34" s="21"/>
@@ -2832,7 +2834,7 @@
       <c r="Z34" s="24"/>
       <c r="AA34" s="21"/>
       <c r="AB34" s="22"/>
-      <c r="AC34" s="115"/>
+      <c r="AC34" s="82"/>
       <c r="AD34" s="70"/>
       <c r="AE34" s="22"/>
       <c r="AF34" s="24"/>
@@ -2856,11 +2858,11 @@
       <c r="M35" s="24"/>
       <c r="N35" s="21"/>
       <c r="O35" s="22"/>
-      <c r="P35" s="77"/>
-      <c r="Q35" s="78"/>
-      <c r="R35" s="78"/>
-      <c r="S35" s="79"/>
-      <c r="T35" s="89"/>
+      <c r="P35" s="107"/>
+      <c r="Q35" s="108"/>
+      <c r="R35" s="108"/>
+      <c r="S35" s="109"/>
+      <c r="T35" s="114"/>
       <c r="U35" s="21"/>
       <c r="V35" s="22"/>
       <c r="W35" s="21"/>
@@ -2869,7 +2871,7 @@
       <c r="Z35" s="24"/>
       <c r="AA35" s="21"/>
       <c r="AB35" s="22"/>
-      <c r="AC35" s="115"/>
+      <c r="AC35" s="82"/>
       <c r="AD35" s="70"/>
       <c r="AE35" s="22"/>
       <c r="AF35" s="24"/>
@@ -2893,11 +2895,11 @@
       <c r="M36" s="24"/>
       <c r="N36" s="21"/>
       <c r="O36" s="22"/>
-      <c r="P36" s="77"/>
-      <c r="Q36" s="78"/>
-      <c r="R36" s="78"/>
-      <c r="S36" s="79"/>
-      <c r="T36" s="89"/>
+      <c r="P36" s="107"/>
+      <c r="Q36" s="108"/>
+      <c r="R36" s="108"/>
+      <c r="S36" s="109"/>
+      <c r="T36" s="114"/>
       <c r="U36" s="21"/>
       <c r="V36" s="22"/>
       <c r="W36" s="21"/>
@@ -2906,7 +2908,7 @@
       <c r="Z36" s="24"/>
       <c r="AA36" s="21"/>
       <c r="AB36" s="22"/>
-      <c r="AC36" s="115"/>
+      <c r="AC36" s="82"/>
       <c r="AD36" s="70"/>
       <c r="AE36" s="22"/>
       <c r="AF36" s="24"/>
@@ -2930,11 +2932,11 @@
       <c r="M37" s="24"/>
       <c r="N37" s="21"/>
       <c r="O37" s="22"/>
-      <c r="P37" s="77"/>
-      <c r="Q37" s="78"/>
-      <c r="R37" s="78"/>
-      <c r="S37" s="79"/>
-      <c r="T37" s="89"/>
+      <c r="P37" s="107"/>
+      <c r="Q37" s="108"/>
+      <c r="R37" s="108"/>
+      <c r="S37" s="109"/>
+      <c r="T37" s="114"/>
       <c r="U37" s="21"/>
       <c r="V37" s="22"/>
       <c r="W37" s="21"/>
@@ -2943,7 +2945,7 @@
       <c r="Z37" s="24"/>
       <c r="AA37" s="21"/>
       <c r="AB37" s="22"/>
-      <c r="AC37" s="115"/>
+      <c r="AC37" s="82"/>
       <c r="AD37" s="70"/>
       <c r="AE37" s="22"/>
       <c r="AF37" s="24"/>
@@ -2967,11 +2969,11 @@
       <c r="M38" s="69"/>
       <c r="N38" s="21"/>
       <c r="O38" s="22"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="78"/>
-      <c r="R38" s="78"/>
-      <c r="S38" s="79"/>
-      <c r="T38" s="89"/>
+      <c r="P38" s="107"/>
+      <c r="Q38" s="108"/>
+      <c r="R38" s="108"/>
+      <c r="S38" s="109"/>
+      <c r="T38" s="114"/>
       <c r="U38" s="21"/>
       <c r="V38" s="68"/>
       <c r="W38" s="21"/>
@@ -3004,11 +3006,11 @@
       <c r="M39" s="69"/>
       <c r="N39" s="21"/>
       <c r="O39" s="22"/>
-      <c r="P39" s="77"/>
-      <c r="Q39" s="78"/>
-      <c r="R39" s="78"/>
-      <c r="S39" s="79"/>
-      <c r="T39" s="89"/>
+      <c r="P39" s="107"/>
+      <c r="Q39" s="108"/>
+      <c r="R39" s="108"/>
+      <c r="S39" s="109"/>
+      <c r="T39" s="114"/>
       <c r="U39" s="21"/>
       <c r="V39" s="68"/>
       <c r="W39" s="21"/>
@@ -3041,11 +3043,11 @@
       <c r="M40" s="24"/>
       <c r="N40" s="21"/>
       <c r="O40" s="22"/>
-      <c r="P40" s="77"/>
-      <c r="Q40" s="78"/>
-      <c r="R40" s="78"/>
-      <c r="S40" s="79"/>
-      <c r="T40" s="89"/>
+      <c r="P40" s="107"/>
+      <c r="Q40" s="108"/>
+      <c r="R40" s="108"/>
+      <c r="S40" s="109"/>
+      <c r="T40" s="114"/>
       <c r="U40" s="21"/>
       <c r="V40" s="22"/>
       <c r="W40" s="21"/>
@@ -3082,11 +3084,11 @@
       <c r="M41" s="46"/>
       <c r="N41" s="41"/>
       <c r="O41" s="44"/>
-      <c r="P41" s="77"/>
-      <c r="Q41" s="78"/>
-      <c r="R41" s="78"/>
-      <c r="S41" s="79"/>
-      <c r="T41" s="89"/>
+      <c r="P41" s="107"/>
+      <c r="Q41" s="108"/>
+      <c r="R41" s="108"/>
+      <c r="S41" s="109"/>
+      <c r="T41" s="114"/>
       <c r="U41" s="41"/>
       <c r="V41" s="44"/>
       <c r="W41" s="41"/>
@@ -3119,11 +3121,11 @@
       <c r="M42" s="66"/>
       <c r="N42" s="41"/>
       <c r="O42" s="44"/>
-      <c r="P42" s="77"/>
-      <c r="Q42" s="78"/>
-      <c r="R42" s="78"/>
-      <c r="S42" s="79"/>
-      <c r="T42" s="89"/>
+      <c r="P42" s="107"/>
+      <c r="Q42" s="108"/>
+      <c r="R42" s="108"/>
+      <c r="S42" s="109"/>
+      <c r="T42" s="114"/>
       <c r="U42" s="41"/>
       <c r="V42" s="44"/>
       <c r="W42" s="41"/>
@@ -3156,11 +3158,11 @@
       <c r="M43" s="67"/>
       <c r="N43" s="26"/>
       <c r="O43" s="27"/>
-      <c r="P43" s="80"/>
-      <c r="Q43" s="81"/>
-      <c r="R43" s="81"/>
-      <c r="S43" s="82"/>
-      <c r="T43" s="90"/>
+      <c r="P43" s="110"/>
+      <c r="Q43" s="111"/>
+      <c r="R43" s="111"/>
+      <c r="S43" s="112"/>
+      <c r="T43" s="115"/>
       <c r="U43" s="26"/>
       <c r="V43" s="27"/>
       <c r="W43" s="26"/>
@@ -3177,6 +3179,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="P6:S43"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="T6:T43"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="AA4:AF4"/>
     <mergeCell ref="H4:M4"/>
@@ -3193,12 +3201,6 @@
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="AC5:AF5"/>
     <mergeCell ref="W5:Z5"/>
-    <mergeCell ref="P6:S43"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="T6:T43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>